<commit_message>
Colocación de codigos para la tesis, fase 1
</commit_message>
<xml_diff>
--- a/facelabels.xlsx
+++ b/facelabels.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\PycharmProjects\FaceMesh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\PycharmProjects\CODIGOS_TESIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A6E133-9A01-4016-9995-BCC7A6136F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD4AFEB-9527-4722-92A8-568C18B2B551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="8" xr2:uid="{4304E637-BFEB-48E3-886B-90B278CDA9D1}"/>
+    <workbookView xWindow="5340" yWindow="5340" windowWidth="19200" windowHeight="9050" activeTab="8" xr2:uid="{4304E637-BFEB-48E3-886B-90B278CDA9D1}"/>
   </bookViews>
   <sheets>
     <sheet name="divisions" sheetId="1" r:id="rId1"/>
@@ -55490,7 +55490,7 @@
   <dimension ref="A2:A745"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A718" workbookViewId="0">
-      <selection activeCell="H749" sqref="H749"/>
+      <selection activeCell="F725" sqref="F725"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
En este caso el código para captura de fotos, etiquetas y borrado, ya funciona, solo faltan pequeños ajustes
</commit_message>
<xml_diff>
--- a/facelabels.xlsx
+++ b/facelabels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\PycharmProjects\CODIGOS_TESIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0662985-94ED-4F2A-AA15-B1DB1BCF2382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F833D971-FFF5-4D49-87B4-D8334DE347EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="815" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23581,7 +23581,7 @@
   <dimension ref="A1:G2083"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2075" workbookViewId="0">
-      <selection activeCell="O2099" sqref="O2099"/>
+      <selection activeCell="Q2099" sqref="Q2099"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Lista la interfaz completa, únicamente falta mejorar la simulación de prediccion, para una mejor visualización
</commit_message>
<xml_diff>
--- a/facelabels.xlsx
+++ b/facelabels.xlsx
@@ -71538,10 +71538,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G748"/>
+  <dimension ref="A1:G745"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A733" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H12"/>
+    <sheetView tabSelected="1" topLeftCell="A736" workbookViewId="0">
+      <selection activeCell="I747" sqref="I747"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -88695,21 +88695,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="746">
-      <c r="G746" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="747">
-      <c r="G747" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="748">
-      <c r="G748" t="n">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Había un problema con la lectura de columnas de excel, ya se solucionó
</commit_message>
<xml_diff>
--- a/facelabels.xlsx
+++ b/facelabels.xlsx
@@ -23596,7 +23596,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2083"/>
+  <dimension ref="A1:G2121"/>
   <sheetViews>
     <sheetView topLeftCell="A2075" workbookViewId="0">
       <selection activeCell="Q2099" sqref="Q2099"/>
@@ -71526,6 +71526,120 @@
       <c r="G2083" t="n">
         <v>2</v>
       </c>
+    </row>
+    <row r="2084">
+      <c r="G2084" t="inlineStr"/>
+    </row>
+    <row r="2085">
+      <c r="G2085" t="inlineStr"/>
+    </row>
+    <row r="2086">
+      <c r="G2086" t="inlineStr"/>
+    </row>
+    <row r="2087">
+      <c r="G2087" t="inlineStr"/>
+    </row>
+    <row r="2088">
+      <c r="G2088" t="inlineStr"/>
+    </row>
+    <row r="2089">
+      <c r="G2089" t="inlineStr"/>
+    </row>
+    <row r="2090">
+      <c r="G2090" t="inlineStr"/>
+    </row>
+    <row r="2091">
+      <c r="G2091" t="inlineStr"/>
+    </row>
+    <row r="2092">
+      <c r="G2092" t="inlineStr"/>
+    </row>
+    <row r="2093">
+      <c r="G2093" t="inlineStr"/>
+    </row>
+    <row r="2094">
+      <c r="G2094" t="inlineStr"/>
+    </row>
+    <row r="2095">
+      <c r="G2095" t="inlineStr"/>
+    </row>
+    <row r="2096">
+      <c r="G2096" t="inlineStr"/>
+    </row>
+    <row r="2097">
+      <c r="G2097" t="inlineStr"/>
+    </row>
+    <row r="2098">
+      <c r="G2098" t="inlineStr"/>
+    </row>
+    <row r="2099">
+      <c r="G2099" t="inlineStr"/>
+    </row>
+    <row r="2100">
+      <c r="G2100" t="inlineStr"/>
+    </row>
+    <row r="2101">
+      <c r="G2101" t="inlineStr"/>
+    </row>
+    <row r="2102">
+      <c r="G2102" t="inlineStr"/>
+    </row>
+    <row r="2103">
+      <c r="G2103" t="inlineStr"/>
+    </row>
+    <row r="2104">
+      <c r="G2104" t="inlineStr"/>
+    </row>
+    <row r="2105">
+      <c r="G2105" t="inlineStr"/>
+    </row>
+    <row r="2106">
+      <c r="G2106" t="inlineStr"/>
+    </row>
+    <row r="2107">
+      <c r="G2107" t="inlineStr"/>
+    </row>
+    <row r="2108">
+      <c r="G2108" t="inlineStr"/>
+    </row>
+    <row r="2109">
+      <c r="G2109" t="inlineStr"/>
+    </row>
+    <row r="2110">
+      <c r="G2110" t="inlineStr"/>
+    </row>
+    <row r="2111">
+      <c r="G2111" t="inlineStr"/>
+    </row>
+    <row r="2112">
+      <c r="G2112" t="inlineStr"/>
+    </row>
+    <row r="2113">
+      <c r="G2113" t="inlineStr"/>
+    </row>
+    <row r="2114">
+      <c r="G2114" t="inlineStr"/>
+    </row>
+    <row r="2115">
+      <c r="G2115" t="inlineStr"/>
+    </row>
+    <row r="2116">
+      <c r="G2116" t="inlineStr"/>
+    </row>
+    <row r="2117">
+      <c r="G2117" t="inlineStr"/>
+    </row>
+    <row r="2118">
+      <c r="G2118" t="inlineStr"/>
+    </row>
+    <row r="2119">
+      <c r="G2119" t="inlineStr"/>
+    </row>
+    <row r="2120">
+      <c r="G2120" t="inlineStr"/>
+    </row>
+    <row r="2121">
+      <c r="G2121" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solo falta arreglar porque Turtle solo funciona 1 vez, lo demás funciona al 100
</commit_message>
<xml_diff>
--- a/facelabels.xlsx
+++ b/facelabels.xlsx
@@ -23596,7 +23596,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2121"/>
+  <dimension ref="A1:G2149"/>
   <sheetViews>
     <sheetView topLeftCell="A2075" workbookViewId="0">
       <selection activeCell="Q2099" sqref="Q2099"/>
@@ -71528,118 +71528,334 @@
       </c>
     </row>
     <row r="2084">
-      <c r="G2084" t="inlineStr"/>
+      <c r="G2084" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2085">
-      <c r="G2085" t="inlineStr"/>
+      <c r="G2085" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2086">
-      <c r="G2086" t="inlineStr"/>
+      <c r="G2086" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2087">
-      <c r="G2087" t="inlineStr"/>
+      <c r="G2087" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2088">
-      <c r="G2088" t="inlineStr"/>
+      <c r="G2088" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2089">
-      <c r="G2089" t="inlineStr"/>
+      <c r="G2089" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2090">
-      <c r="G2090" t="inlineStr"/>
+      <c r="G2090" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2091">
-      <c r="G2091" t="inlineStr"/>
+      <c r="G2091" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2092">
-      <c r="G2092" t="inlineStr"/>
+      <c r="G2092" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2093">
-      <c r="G2093" t="inlineStr"/>
+      <c r="G2093" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2094">
-      <c r="G2094" t="inlineStr"/>
+      <c r="G2094" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2095">
-      <c r="G2095" t="inlineStr"/>
+      <c r="G2095" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2096">
-      <c r="G2096" t="inlineStr"/>
+      <c r="G2096" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2097">
-      <c r="G2097" t="inlineStr"/>
+      <c r="G2097" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2098">
-      <c r="G2098" t="inlineStr"/>
+      <c r="G2098" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2099">
-      <c r="G2099" t="inlineStr"/>
+      <c r="G2099" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2100">
-      <c r="G2100" t="inlineStr"/>
+      <c r="G2100" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2101">
-      <c r="G2101" t="inlineStr"/>
+      <c r="G2101" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2102">
-      <c r="G2102" t="inlineStr"/>
+      <c r="G2102" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2103">
-      <c r="G2103" t="inlineStr"/>
+      <c r="G2103" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2104">
-      <c r="G2104" t="inlineStr"/>
+      <c r="G2104" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2105">
-      <c r="G2105" t="inlineStr"/>
+      <c r="G2105" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2106">
-      <c r="G2106" t="inlineStr"/>
+      <c r="G2106" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2107">
-      <c r="G2107" t="inlineStr"/>
+      <c r="G2107" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2108">
-      <c r="G2108" t="inlineStr"/>
+      <c r="G2108" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2109">
-      <c r="G2109" t="inlineStr"/>
+      <c r="G2109" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2110">
-      <c r="G2110" t="inlineStr"/>
+      <c r="G2110" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2111">
-      <c r="G2111" t="inlineStr"/>
+      <c r="G2111" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2112">
-      <c r="G2112" t="inlineStr"/>
+      <c r="G2112" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2113">
-      <c r="G2113" t="inlineStr"/>
+      <c r="G2113" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2114">
-      <c r="G2114" t="inlineStr"/>
+      <c r="G2114" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2115">
-      <c r="G2115" t="inlineStr"/>
+      <c r="G2115" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2116">
-      <c r="G2116" t="inlineStr"/>
+      <c r="G2116" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2117">
-      <c r="G2117" t="inlineStr"/>
+      <c r="G2117" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2118">
-      <c r="G2118" t="inlineStr"/>
+      <c r="G2118" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="2119">
-      <c r="G2119" t="inlineStr"/>
+      <c r="G2119" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="2120">
-      <c r="G2120" t="inlineStr"/>
+      <c r="G2120" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="2121">
-      <c r="G2121" t="inlineStr"/>
+      <c r="G2121" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2122">
+      <c r="G2122" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2123">
+      <c r="G2123" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2124">
+      <c r="G2124" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2125">
+      <c r="G2125" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2126">
+      <c r="G2126" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2127">
+      <c r="G2127" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2128">
+      <c r="G2128" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2129">
+      <c r="G2129" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2130">
+      <c r="G2130" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2131">
+      <c r="G2131" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2132">
+      <c r="G2132" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2133">
+      <c r="G2133" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2134">
+      <c r="G2134" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2135">
+      <c r="G2135" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2136">
+      <c r="G2136" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2137">
+      <c r="G2137" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2138">
+      <c r="G2138" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2139">
+      <c r="G2139" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2140">
+      <c r="G2140" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2141">
+      <c r="G2141" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2142">
+      <c r="G2142" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2143">
+      <c r="G2143" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2144">
+      <c r="G2144" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2145">
+      <c r="G2145" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2146">
+      <c r="G2146" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2147">
+      <c r="G2147" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2148">
+      <c r="G2148" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2149">
+      <c r="G2149" t="n">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
PRUEBAS DE FILTROS DE COLOR Y BORDES
</commit_message>
<xml_diff>
--- a/facelabels.xlsx
+++ b/facelabels.xlsx
@@ -23596,7 +23596,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2149"/>
+  <dimension ref="A1:G2160"/>
   <sheetViews>
     <sheetView topLeftCell="A2075" workbookViewId="0">
       <selection activeCell="Q2099" sqref="Q2099"/>
@@ -71579,17 +71579,17 @@
     </row>
     <row r="2094">
       <c r="G2094" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2095">
       <c r="G2095" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2096">
       <c r="G2096" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2097">
@@ -71699,42 +71699,42 @@
     </row>
     <row r="2118">
       <c r="G2118" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2119">
       <c r="G2119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2120">
       <c r="G2120" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2121">
       <c r="G2121" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2122">
       <c r="G2122" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2123">
       <c r="G2123" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2124">
       <c r="G2124" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2125">
       <c r="G2125" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2126">
@@ -71764,47 +71764,47 @@
     </row>
     <row r="2131">
       <c r="G2131" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2132">
       <c r="G2132" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2133">
       <c r="G2133" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2134">
       <c r="G2134" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2135">
       <c r="G2135" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2136">
       <c r="G2136" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2137">
       <c r="G2137" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2138">
       <c r="G2138" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2139">
       <c r="G2139" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2140">
@@ -71854,6 +71854,61 @@
     </row>
     <row r="2149">
       <c r="G2149" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2150">
+      <c r="G2150" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2151">
+      <c r="G2151" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2152">
+      <c r="G2152" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2153">
+      <c r="G2153" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2154">
+      <c r="G2154" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2155">
+      <c r="G2155" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2156">
+      <c r="G2156" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2157">
+      <c r="G2157" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2158">
+      <c r="G2158" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2159">
+      <c r="G2159" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2160">
+      <c r="G2160" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ahora ya se guardan los landmarks en formato de npy
</commit_message>
<xml_diff>
--- a/facelabels.xlsx
+++ b/facelabels.xlsx
@@ -23596,10 +23596,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2834"/>
+  <dimension ref="A1:M2834"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -23650,6 +23650,11 @@
           <t>M8</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>M9</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -23679,11 +23684,12 @@
       <c r="I2" t="n">
         <v>1</v>
       </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <f>COUNTIF($I$2084:$I$2761,K2)</f>
+      <c r="J2" t="inlineStr"/>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f>COUNTIF($I$2084:$I$2761,L2)</f>
         <v/>
       </c>
     </row>
@@ -23715,11 +23721,12 @@
       <c r="I3" t="n">
         <v>0</v>
       </c>
-      <c r="K3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <f>COUNTIF($I$2084:$I$2761,K3)</f>
+      <c r="J3" t="inlineStr"/>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <f>COUNTIF($I$2084:$I$2761,L3)</f>
         <v/>
       </c>
     </row>
@@ -23751,11 +23758,12 @@
       <c r="I4" t="n">
         <v>0</v>
       </c>
-      <c r="K4" t="n">
-        <v>2</v>
-      </c>
-      <c r="L4">
-        <f>COUNTIF($I$2084:$I$2761,K4)</f>
+      <c r="J4" t="inlineStr"/>
+      <c r="L4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <f>COUNTIF($I$2084:$I$2761,L4)</f>
         <v/>
       </c>
     </row>
@@ -23787,11 +23795,12 @@
       <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="K5" t="n">
-        <v>3</v>
-      </c>
-      <c r="L5">
-        <f>COUNTIF($I$2084:$I$2761,K5)</f>
+      <c r="J5" t="inlineStr"/>
+      <c r="L5" t="n">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <f>COUNTIF($I$2084:$I$2761,L5)</f>
         <v/>
       </c>
     </row>
@@ -23823,6 +23832,7 @@
       <c r="I6" t="n">
         <v>0</v>
       </c>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -23852,6 +23862,7 @@
       <c r="I7" t="n">
         <v>0</v>
       </c>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -23881,6 +23892,7 @@
       <c r="I8" t="n">
         <v>1</v>
       </c>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -23910,6 +23922,7 @@
       <c r="I9" t="n">
         <v>1</v>
       </c>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -23939,6 +23952,7 @@
       <c r="I10" t="n">
         <v>1</v>
       </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -23968,6 +23982,7 @@
       <c r="I11" t="n">
         <v>2</v>
       </c>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -23997,6 +24012,7 @@
       <c r="I12" t="n">
         <v>2</v>
       </c>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -24026,6 +24042,7 @@
       <c r="I13" t="n">
         <v>2</v>
       </c>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -24055,6 +24072,7 @@
       <c r="I14" t="n">
         <v>2</v>
       </c>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -24084,6 +24102,7 @@
       <c r="I15" t="n">
         <v>2</v>
       </c>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -24113,6 +24132,7 @@
       <c r="I16" t="n">
         <v>0</v>
       </c>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -24142,6 +24162,7 @@
       <c r="I17" t="n">
         <v>0</v>
       </c>
+      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -24171,6 +24192,7 @@
       <c r="I18" t="n">
         <v>0</v>
       </c>
+      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -24200,6 +24222,7 @@
       <c r="I19" t="n">
         <v>0</v>
       </c>
+      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -24229,6 +24252,7 @@
       <c r="I20" t="n">
         <v>0</v>
       </c>
+      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -24258,6 +24282,7 @@
       <c r="I21" t="n">
         <v>1</v>
       </c>
+      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -24287,6 +24312,7 @@
       <c r="I22" t="n">
         <v>1</v>
       </c>
+      <c r="J22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -24316,6 +24342,7 @@
       <c r="I23" t="n">
         <v>1</v>
       </c>
+      <c r="J23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -24345,6 +24372,7 @@
       <c r="I24" t="n">
         <v>2</v>
       </c>
+      <c r="J24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -24374,6 +24402,7 @@
       <c r="I25" t="n">
         <v>2</v>
       </c>
+      <c r="J25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -24403,6 +24432,7 @@
       <c r="I26" t="n">
         <v>2</v>
       </c>
+      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -24432,6 +24462,7 @@
       <c r="I27" t="n">
         <v>2</v>
       </c>
+      <c r="J27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -24461,6 +24492,7 @@
       <c r="I28" t="n">
         <v>2</v>
       </c>
+      <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -24490,6 +24522,7 @@
       <c r="I29" t="n">
         <v>0</v>
       </c>
+      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -24519,6 +24552,7 @@
       <c r="I30" t="n">
         <v>0</v>
       </c>
+      <c r="J30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -24548,6 +24582,7 @@
       <c r="I31" t="n">
         <v>0</v>
       </c>
+      <c r="J31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -24577,6 +24612,7 @@
       <c r="I32" t="n">
         <v>0</v>
       </c>
+      <c r="J32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -24606,6 +24642,7 @@
       <c r="I33" t="n">
         <v>0</v>
       </c>
+      <c r="J33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -24635,6 +24672,7 @@
       <c r="I34" t="n">
         <v>1</v>
       </c>
+      <c r="J34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -24664,6 +24702,7 @@
       <c r="I35" t="n">
         <v>1</v>
       </c>
+      <c r="J35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -24693,6 +24732,7 @@
       <c r="I36" t="n">
         <v>1</v>
       </c>
+      <c r="J36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -24722,6 +24762,7 @@
       <c r="I37" t="n">
         <v>2</v>
       </c>
+      <c r="J37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -24751,6 +24792,7 @@
       <c r="I38" t="n">
         <v>2</v>
       </c>
+      <c r="J38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -24780,6 +24822,7 @@
       <c r="I39" t="n">
         <v>2</v>
       </c>
+      <c r="J39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -24809,6 +24852,7 @@
       <c r="I40" t="n">
         <v>2</v>
       </c>
+      <c r="J40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -24838,6 +24882,7 @@
       <c r="I41" t="n">
         <v>2</v>
       </c>
+      <c r="J41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -24867,6 +24912,7 @@
       <c r="I42" t="n">
         <v>0</v>
       </c>
+      <c r="J42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -24896,6 +24942,7 @@
       <c r="I43" t="n">
         <v>0</v>
       </c>
+      <c r="J43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -24925,6 +24972,7 @@
       <c r="I44" t="n">
         <v>0</v>
       </c>
+      <c r="J44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -24954,6 +25002,7 @@
       <c r="I45" t="n">
         <v>0</v>
       </c>
+      <c r="J45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -24983,6 +25032,7 @@
       <c r="I46" t="n">
         <v>0</v>
       </c>
+      <c r="J46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -25012,6 +25062,7 @@
       <c r="I47" t="n">
         <v>1</v>
       </c>
+      <c r="J47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -25041,6 +25092,7 @@
       <c r="I48" t="n">
         <v>1</v>
       </c>
+      <c r="J48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -25070,6 +25122,7 @@
       <c r="I49" t="n">
         <v>1</v>
       </c>
+      <c r="J49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -25099,6 +25152,7 @@
       <c r="I50" t="n">
         <v>2</v>
       </c>
+      <c r="J50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -25128,6 +25182,7 @@
       <c r="I51" t="n">
         <v>2</v>
       </c>
+      <c r="J51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -25157,6 +25212,7 @@
       <c r="I52" t="n">
         <v>2</v>
       </c>
+      <c r="J52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -25186,6 +25242,7 @@
       <c r="I53" t="n">
         <v>2</v>
       </c>
+      <c r="J53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -25215,6 +25272,7 @@
       <c r="I54" t="n">
         <v>2</v>
       </c>
+      <c r="J54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -25244,6 +25302,7 @@
       <c r="I55" t="n">
         <v>0</v>
       </c>
+      <c r="J55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -25273,6 +25332,7 @@
       <c r="I56" t="n">
         <v>0</v>
       </c>
+      <c r="J56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -25302,6 +25362,7 @@
       <c r="I57" t="n">
         <v>0</v>
       </c>
+      <c r="J57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -25331,6 +25392,7 @@
       <c r="I58" t="n">
         <v>0</v>
       </c>
+      <c r="J58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -25360,6 +25422,7 @@
       <c r="I59" t="n">
         <v>0</v>
       </c>
+      <c r="J59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -25389,6 +25452,7 @@
       <c r="I60" t="n">
         <v>3</v>
       </c>
+      <c r="J60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -25418,6 +25482,7 @@
       <c r="I61" t="n">
         <v>3</v>
       </c>
+      <c r="J61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -25447,6 +25512,7 @@
       <c r="I62" t="n">
         <v>3</v>
       </c>
+      <c r="J62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -25476,6 +25542,7 @@
       <c r="I63" t="n">
         <v>2</v>
       </c>
+      <c r="J63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -25505,6 +25572,7 @@
       <c r="I64" t="n">
         <v>2</v>
       </c>
+      <c r="J64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -25534,6 +25602,7 @@
       <c r="I65" t="n">
         <v>2</v>
       </c>
+      <c r="J65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -25563,6 +25632,7 @@
       <c r="I66" t="n">
         <v>2</v>
       </c>
+      <c r="J66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -25592,6 +25662,7 @@
       <c r="I67" t="n">
         <v>2</v>
       </c>
+      <c r="J67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -25621,6 +25692,7 @@
       <c r="I68" t="n">
         <v>0</v>
       </c>
+      <c r="J68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -25650,6 +25722,7 @@
       <c r="I69" t="n">
         <v>0</v>
       </c>
+      <c r="J69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -25679,6 +25752,7 @@
       <c r="I70" t="n">
         <v>0</v>
       </c>
+      <c r="J70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -25708,6 +25782,7 @@
       <c r="I71" t="n">
         <v>0</v>
       </c>
+      <c r="J71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -25737,6 +25812,7 @@
       <c r="I72" t="n">
         <v>3</v>
       </c>
+      <c r="J72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -25766,6 +25842,7 @@
       <c r="I73" t="n">
         <v>3</v>
       </c>
+      <c r="J73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -25795,6 +25872,7 @@
       <c r="I74" t="n">
         <v>3</v>
       </c>
+      <c r="J74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -25824,6 +25902,7 @@
       <c r="I75" t="n">
         <v>3</v>
       </c>
+      <c r="J75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -25853,6 +25932,7 @@
       <c r="I76" t="n">
         <v>3</v>
       </c>
+      <c r="J76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -25882,6 +25962,7 @@
       <c r="I77" t="n">
         <v>2</v>
       </c>
+      <c r="J77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -25911,6 +25992,7 @@
       <c r="I78" t="n">
         <v>2</v>
       </c>
+      <c r="J78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -25940,6 +26022,7 @@
       <c r="I79" t="n">
         <v>2</v>
       </c>
+      <c r="J79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -25969,6 +26052,7 @@
       <c r="I80" t="n">
         <v>2</v>
       </c>
+      <c r="J80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -25998,6 +26082,7 @@
       <c r="I81" t="n">
         <v>0</v>
       </c>
+      <c r="J81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -26027,6 +26112,7 @@
       <c r="I82" t="n">
         <v>0</v>
       </c>
+      <c r="J82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -26056,6 +26142,7 @@
       <c r="I83" t="n">
         <v>0</v>
       </c>
+      <c r="J83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -26085,6 +26172,7 @@
       <c r="I84" t="n">
         <v>0</v>
       </c>
+      <c r="J84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -26114,6 +26202,7 @@
       <c r="I85" t="n">
         <v>3</v>
       </c>
+      <c r="J85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -26143,6 +26232,7 @@
       <c r="I86" t="n">
         <v>3</v>
       </c>
+      <c r="J86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -26172,6 +26262,7 @@
       <c r="I87" t="n">
         <v>3</v>
       </c>
+      <c r="J87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -26201,6 +26292,7 @@
       <c r="I88" t="n">
         <v>3</v>
       </c>
+      <c r="J88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -26230,6 +26322,7 @@
       <c r="I89" t="n">
         <v>3</v>
       </c>
+      <c r="J89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -26259,6 +26352,7 @@
       <c r="I90" t="n">
         <v>2</v>
       </c>
+      <c r="J90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -26288,6 +26382,7 @@
       <c r="I91" t="n">
         <v>2</v>
       </c>
+      <c r="J91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -26317,6 +26412,7 @@
       <c r="I92" t="n">
         <v>2</v>
       </c>
+      <c r="J92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -26346,6 +26442,7 @@
       <c r="I93" t="n">
         <v>2</v>
       </c>
+      <c r="J93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -26375,6 +26472,7 @@
       <c r="I94" t="n">
         <v>3</v>
       </c>
+      <c r="J94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -26404,6 +26502,7 @@
       <c r="I95" t="n">
         <v>1</v>
       </c>
+      <c r="J95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -26433,6 +26532,7 @@
       <c r="I96" t="n">
         <v>0</v>
       </c>
+      <c r="J96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -26462,6 +26562,7 @@
       <c r="I97" t="n">
         <v>0</v>
       </c>
+      <c r="J97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -26491,6 +26592,7 @@
       <c r="I98" t="n">
         <v>0</v>
       </c>
+      <c r="J98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -26520,6 +26622,7 @@
       <c r="I99" t="n">
         <v>0</v>
       </c>
+      <c r="J99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -26549,6 +26652,7 @@
       <c r="I100" t="n">
         <v>0</v>
       </c>
+      <c r="J100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -26578,6 +26682,7 @@
       <c r="I101" t="n">
         <v>1</v>
       </c>
+      <c r="J101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -26607,6 +26712,7 @@
       <c r="I102" t="n">
         <v>1</v>
       </c>
+      <c r="J102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -26636,6 +26742,7 @@
       <c r="I103" t="n">
         <v>1</v>
       </c>
+      <c r="J103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -26665,6 +26772,7 @@
       <c r="I104" t="n">
         <v>2</v>
       </c>
+      <c r="J104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -26694,6 +26802,7 @@
       <c r="I105" t="n">
         <v>2</v>
       </c>
+      <c r="J105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -26723,6 +26832,7 @@
       <c r="I106" t="n">
         <v>2</v>
       </c>
+      <c r="J106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -26752,6 +26862,7 @@
       <c r="I107" t="n">
         <v>2</v>
       </c>
+      <c r="J107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -26781,6 +26892,7 @@
       <c r="I108" t="n">
         <v>2</v>
       </c>
+      <c r="J108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -26810,6 +26922,7 @@
       <c r="I109" t="n">
         <v>0</v>
       </c>
+      <c r="J109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -26839,6 +26952,7 @@
       <c r="I110" t="n">
         <v>0</v>
       </c>
+      <c r="J110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -26868,6 +26982,7 @@
       <c r="I111" t="n">
         <v>0</v>
       </c>
+      <c r="J111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -26897,6 +27012,7 @@
       <c r="I112" t="n">
         <v>0</v>
       </c>
+      <c r="J112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -26926,6 +27042,7 @@
       <c r="I113" t="n">
         <v>0</v>
       </c>
+      <c r="J113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -26955,6 +27072,7 @@
       <c r="I114" t="n">
         <v>1</v>
       </c>
+      <c r="J114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -26984,6 +27102,7 @@
       <c r="I115" t="n">
         <v>1</v>
       </c>
+      <c r="J115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -27013,6 +27132,7 @@
       <c r="I116" t="n">
         <v>1</v>
       </c>
+      <c r="J116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -27042,6 +27162,7 @@
       <c r="I117" t="n">
         <v>2</v>
       </c>
+      <c r="J117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -27071,6 +27192,7 @@
       <c r="I118" t="n">
         <v>2</v>
       </c>
+      <c r="J118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -27100,6 +27222,7 @@
       <c r="I119" t="n">
         <v>2</v>
       </c>
+      <c r="J119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -27129,6 +27252,7 @@
       <c r="I120" t="n">
         <v>2</v>
       </c>
+      <c r="J120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -27158,6 +27282,7 @@
       <c r="I121" t="n">
         <v>2</v>
       </c>
+      <c r="J121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -27187,6 +27312,7 @@
       <c r="I122" t="n">
         <v>0</v>
       </c>
+      <c r="J122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -27216,6 +27342,7 @@
       <c r="I123" t="n">
         <v>0</v>
       </c>
+      <c r="J123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -27245,6 +27372,7 @@
       <c r="I124" t="n">
         <v>0</v>
       </c>
+      <c r="J124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -27274,6 +27402,7 @@
       <c r="I125" t="n">
         <v>0</v>
       </c>
+      <c r="J125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -27303,6 +27432,7 @@
       <c r="I126" t="n">
         <v>0</v>
       </c>
+      <c r="J126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -27332,6 +27462,7 @@
       <c r="I127" t="n">
         <v>1</v>
       </c>
+      <c r="J127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -27361,6 +27492,7 @@
       <c r="I128" t="n">
         <v>1</v>
       </c>
+      <c r="J128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -27390,6 +27522,7 @@
       <c r="I129" t="n">
         <v>1</v>
       </c>
+      <c r="J129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -27419,6 +27552,7 @@
       <c r="I130" t="n">
         <v>2</v>
       </c>
+      <c r="J130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -27448,6 +27582,7 @@
       <c r="I131" t="n">
         <v>2</v>
       </c>
+      <c r="J131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -27477,6 +27612,7 @@
       <c r="I132" t="n">
         <v>2</v>
       </c>
+      <c r="J132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -27506,6 +27642,7 @@
       <c r="I133" t="n">
         <v>2</v>
       </c>
+      <c r="J133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -27535,6 +27672,7 @@
       <c r="I134" t="n">
         <v>2</v>
       </c>
+      <c r="J134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -27564,6 +27702,7 @@
       <c r="I135" t="n">
         <v>0</v>
       </c>
+      <c r="J135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -27593,6 +27732,7 @@
       <c r="I136" t="n">
         <v>0</v>
       </c>
+      <c r="J136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -27622,6 +27762,7 @@
       <c r="I137" t="n">
         <v>0</v>
       </c>
+      <c r="J137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -27651,6 +27792,7 @@
       <c r="I138" t="n">
         <v>0</v>
       </c>
+      <c r="J138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -27680,6 +27822,7 @@
       <c r="I139" t="n">
         <v>0</v>
       </c>
+      <c r="J139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -27709,6 +27852,7 @@
       <c r="I140" t="n">
         <v>1</v>
       </c>
+      <c r="J140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -27738,6 +27882,7 @@
       <c r="I141" t="n">
         <v>1</v>
       </c>
+      <c r="J141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -27767,6 +27912,7 @@
       <c r="I142" t="n">
         <v>1</v>
       </c>
+      <c r="J142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -27796,6 +27942,7 @@
       <c r="I143" t="n">
         <v>2</v>
       </c>
+      <c r="J143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -27825,6 +27972,7 @@
       <c r="I144" t="n">
         <v>2</v>
       </c>
+      <c r="J144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -27854,6 +28002,7 @@
       <c r="I145" t="n">
         <v>2</v>
       </c>
+      <c r="J145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -27883,6 +28032,7 @@
       <c r="I146" t="n">
         <v>2</v>
       </c>
+      <c r="J146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -27912,6 +28062,7 @@
       <c r="I147" t="n">
         <v>2</v>
       </c>
+      <c r="J147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -27941,6 +28092,7 @@
       <c r="I148" t="n">
         <v>0</v>
       </c>
+      <c r="J148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -27970,6 +28122,7 @@
       <c r="I149" t="n">
         <v>0</v>
       </c>
+      <c r="J149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -27999,6 +28152,7 @@
       <c r="I150" t="n">
         <v>0</v>
       </c>
+      <c r="J150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -28028,6 +28182,7 @@
       <c r="I151" t="n">
         <v>0</v>
       </c>
+      <c r="J151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -28057,6 +28212,7 @@
       <c r="I152" t="n">
         <v>0</v>
       </c>
+      <c r="J152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -28086,6 +28242,7 @@
       <c r="I153" t="n">
         <v>3</v>
       </c>
+      <c r="J153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -28115,6 +28272,7 @@
       <c r="I154" t="n">
         <v>3</v>
       </c>
+      <c r="J154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -28144,6 +28302,7 @@
       <c r="I155" t="n">
         <v>3</v>
       </c>
+      <c r="J155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -28173,6 +28332,7 @@
       <c r="I156" t="n">
         <v>2</v>
       </c>
+      <c r="J156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -28202,6 +28362,7 @@
       <c r="I157" t="n">
         <v>2</v>
       </c>
+      <c r="J157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -28231,6 +28392,7 @@
       <c r="I158" t="n">
         <v>2</v>
       </c>
+      <c r="J158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -28260,6 +28422,7 @@
       <c r="I159" t="n">
         <v>2</v>
       </c>
+      <c r="J159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -28289,6 +28452,7 @@
       <c r="I160" t="n">
         <v>2</v>
       </c>
+      <c r="J160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -28318,6 +28482,7 @@
       <c r="I161" t="n">
         <v>0</v>
       </c>
+      <c r="J161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -28347,6 +28512,7 @@
       <c r="I162" t="n">
         <v>0</v>
       </c>
+      <c r="J162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="n">
@@ -28376,6 +28542,7 @@
       <c r="I163" t="n">
         <v>0</v>
       </c>
+      <c r="J163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -28405,6 +28572,7 @@
       <c r="I164" t="n">
         <v>0</v>
       </c>
+      <c r="J164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -28434,6 +28602,7 @@
       <c r="I165" t="n">
         <v>3</v>
       </c>
+      <c r="J165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -28463,6 +28632,7 @@
       <c r="I166" t="n">
         <v>3</v>
       </c>
+      <c r="J166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -28492,6 +28662,7 @@
       <c r="I167" t="n">
         <v>3</v>
       </c>
+      <c r="J167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -28521,6 +28692,7 @@
       <c r="I168" t="n">
         <v>3</v>
       </c>
+      <c r="J168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -28550,6 +28722,7 @@
       <c r="I169" t="n">
         <v>3</v>
       </c>
+      <c r="J169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -28579,6 +28752,7 @@
       <c r="I170" t="n">
         <v>2</v>
       </c>
+      <c r="J170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="n">
@@ -88057,7 +88231,7 @@
   <dimension ref="A1:M1035"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -88108,6 +88282,11 @@
           <t>M8</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>M9</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">

</xml_diff>

<commit_message>
Ahora, no se necesita el archivo extractData, se hará dicha extracción en el codigo del modelo
</commit_message>
<xml_diff>
--- a/facelabels.xlsx
+++ b/facelabels.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="815" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="815" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="divisions" sheetId="1" state="visible" r:id="rId1"/>
@@ -23598,8 +23598,8 @@
   </sheetPr>
   <dimension ref="A1:M2834"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -27329,7 +27329,7 @@
         <v>1</v>
       </c>
       <c r="J115" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -27361,7 +27361,7 @@
         <v>1</v>
       </c>
       <c r="J116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117">
@@ -27393,7 +27393,7 @@
         <v>2</v>
       </c>
       <c r="J117" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118">
@@ -31073,7 +31073,7 @@
         <v>0</v>
       </c>
       <c r="J232" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="233">
@@ -31105,7 +31105,7 @@
         <v>1</v>
       </c>
       <c r="J233" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="234">
@@ -31137,7 +31137,7 @@
         <v>1</v>
       </c>
       <c r="J234" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="235">
@@ -34881,7 +34881,7 @@
         <v>3</v>
       </c>
       <c r="J351" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="352">
@@ -38656,6 +38656,9 @@
       <c r="I469" t="n">
         <v>0</v>
       </c>
+      <c r="J469" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="470">
       <c r="A470" t="n">
@@ -38684,6 +38687,9 @@
       </c>
       <c r="I470" t="n">
         <v>0</v>
+      </c>
+      <c r="J470" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="471">
@@ -89462,8 +89468,8 @@
   </sheetPr>
   <dimension ref="A1:M1035"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -91049,7 +91055,7 @@
         <v>1</v>
       </c>
       <c r="J48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -91081,7 +91087,7 @@
         <v>1</v>
       </c>
       <c r="J49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -91113,7 +91119,7 @@
         <v>2</v>
       </c>
       <c r="J50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -92585,7 +92591,7 @@
         <v>0</v>
       </c>
       <c r="J96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -92617,7 +92623,7 @@
         <v>0</v>
       </c>
       <c r="J97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -92649,7 +92655,7 @@
         <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -92681,7 +92687,7 @@
         <v>0</v>
       </c>
       <c r="J99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -92713,7 +92719,7 @@
         <v>0</v>
       </c>
       <c r="J100" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -94153,7 +94159,7 @@
         <v>2</v>
       </c>
       <c r="J145" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146">
@@ -94185,7 +94191,7 @@
         <v>2</v>
       </c>
       <c r="J146" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147">
@@ -94217,7 +94223,7 @@
         <v>2</v>
       </c>
       <c r="J147" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148">
@@ -94249,7 +94255,7 @@
         <v>0</v>
       </c>
       <c r="J148" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149">
@@ -94281,7 +94287,7 @@
         <v>0</v>
       </c>
       <c r="J149" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150">
@@ -94313,7 +94319,7 @@
         <v>0</v>
       </c>
       <c r="J150" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151">
@@ -95688,6 +95694,9 @@
       <c r="I193" t="n">
         <v>0</v>
       </c>
+      <c r="J193" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
@@ -95717,6 +95726,9 @@
       <c r="I194" t="n">
         <v>1</v>
       </c>
+      <c r="J194" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
@@ -95746,6 +95758,9 @@
       <c r="I195" t="n">
         <v>1</v>
       </c>
+      <c r="J195" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
@@ -95775,6 +95790,9 @@
       <c r="I196" t="n">
         <v>1</v>
       </c>
+      <c r="J196" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
@@ -95804,6 +95822,9 @@
       <c r="I197" t="n">
         <v>2</v>
       </c>
+      <c r="J197" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
@@ -95833,6 +95854,9 @@
       <c r="I198" t="n">
         <v>2</v>
       </c>
+      <c r="J198" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
@@ -95862,6 +95886,9 @@
       <c r="I199" t="n">
         <v>2</v>
       </c>
+      <c r="J199" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
@@ -95890,6 +95917,9 @@
       </c>
       <c r="I200" t="n">
         <v>2</v>
+      </c>
+      <c r="J200" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="201">

</xml_diff>